<commit_message>
armor augment data sheet
</commit_message>
<xml_diff>
--- a/misc/ArmorAugmentSheet.xlsx
+++ b/misc/ArmorAugmentSheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\InhaGame-2024\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JooWoan-WorkSpace\InhaGame-2024\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CA5BF1-AD95-4238-AF59-085609811685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="225" windowWidth="27720" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="345" yWindow="255" windowWidth="27720" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,7 +109,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -680,12 +681,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -737,16 +738,16 @@
         <v>10</v>
       </c>
       <c r="D3" s="9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E3" s="10">
         <v>10</v>
       </c>
       <c r="F3" s="9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G3" s="10">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -756,16 +757,16 @@
         <v>11</v>
       </c>
       <c r="D4" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E4" s="12">
         <v>10</v>
       </c>
       <c r="F4" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G4" s="12">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -775,16 +776,16 @@
         <v>12</v>
       </c>
       <c r="D5" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E5" s="12">
         <v>10</v>
       </c>
       <c r="F5" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G5" s="12">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -794,16 +795,16 @@
         <v>13</v>
       </c>
       <c r="D6" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E6" s="12">
         <v>10</v>
       </c>
       <c r="F6" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G6" s="12">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -813,16 +814,16 @@
         <v>14</v>
       </c>
       <c r="D7" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E7" s="12">
         <v>10</v>
       </c>
       <c r="F7" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G7" s="12">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -834,16 +835,16 @@
         <v>4</v>
       </c>
       <c r="D8" s="9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E8" s="10">
         <v>10</v>
       </c>
       <c r="F8" s="9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G8" s="10">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -853,16 +854,16 @@
         <v>15</v>
       </c>
       <c r="D9" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E9" s="12">
         <v>10</v>
       </c>
       <c r="F9" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G9" s="12">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -872,16 +873,16 @@
         <v>3</v>
       </c>
       <c r="D10" s="13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E10" s="14">
         <v>10</v>
       </c>
       <c r="F10" s="13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G10" s="14">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -893,16 +894,16 @@
         <v>16</v>
       </c>
       <c r="D11" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E11" s="12">
         <v>10</v>
       </c>
       <c r="F11" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G11" s="12">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -912,16 +913,16 @@
         <v>7</v>
       </c>
       <c r="D12" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E12" s="12">
         <v>10</v>
       </c>
       <c r="F12" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G12" s="12">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -931,16 +932,16 @@
         <v>17</v>
       </c>
       <c r="D13" s="13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E13" s="14">
         <v>10</v>
       </c>
       <c r="F13" s="13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G13" s="14">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>